<commit_message>
third teams tie break
</commit_message>
<xml_diff>
--- a/data/out/wiki/men/fifa/eu/best_four_third_teams_eu_fifa.xlsx
+++ b/data/out/wiki/men/fifa/eu/best_four_third_teams_eu_fifa.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -509,12 +509,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['Northern Ireland', 'Portugal', 'Romania', 'Slovakia']</t>
+          <t>['Czech Republic', 'Northern Ireland', 'Portugal', 'Slovakia']</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Sweden']</t>
+          <t>['Romania', 'Sweden']</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -568,12 +568,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['Northern Ireland', 'Portugal', 'Romania', 'Slovakia']</t>
+          <t>['Czech Republic', 'Northern Ireland', 'Portugal', 'Slovakia']</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Sweden']</t>
+          <t>['Romania', 'Sweden']</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -809,7 +809,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>['Sweden', 'Portugal']</t>
+          <t>['Portugal', 'Sweden']</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -868,7 +868,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>['Sweden', 'Portugal']</t>
+          <t>['Portugal', 'Sweden']</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -927,7 +927,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>['Sweden', 'Portugal']</t>
+          <t>['Portugal', 'Sweden']</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">

</xml_diff>